<commit_message>
Added color identifiers for tests on spreadsheet
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blaze\Desktop\SW-ENG\ClueGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John Klassen\eclipse-workspace\ClueGameSW\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6F72D94-F6B4-4420-BC23-85AF8CD84876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99CB2C3-4DA0-4A3C-B01D-E8700C013F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-86" yWindow="0" windowWidth="14983" windowHeight="17880" xr2:uid="{458EB856-E50E-4072-8F58-AC2C0DAFB3C4}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="17550" xr2:uid="{458EB856-E50E-4072-8F58-AC2C0DAFB3C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="42">
   <si>
     <t>W</t>
   </si>
@@ -141,13 +141,34 @@
   </si>
   <si>
     <t>BK</t>
+  </si>
+  <si>
+    <t>Number of doors: 17</t>
+  </si>
+  <si>
+    <t>Grey: room test (in FileInitTest</t>
+  </si>
+  <si>
+    <t>White: door direction tests (in FileInitTest)</t>
+  </si>
+  <si>
+    <t>Light Blue: adjacency from rooms and doors</t>
+  </si>
+  <si>
+    <t>Green: adjacencywalkways</t>
+  </si>
+  <si>
+    <t>Red - Test Occupied</t>
+  </si>
+  <si>
+    <t>Black - Test Targets</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,8 +199,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,8 +258,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -246,11 +318,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -277,6 +369,41 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -618,18 +745,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E9A66F2-46E9-4D9D-A0FD-4154B91B0CA4}">
-  <dimension ref="A1:Y27"/>
+  <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="25" width="4.69140625" customWidth="1"/>
+    <col min="1" max="25" width="4.7109375" customWidth="1"/>
+    <col min="27" max="27" width="41.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2">
         <v>0</v>
@@ -703,8 +831,11 @@
       <c r="Y1" s="2">
         <v>22</v>
       </c>
+      <c r="AA1" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -780,8 +911,11 @@
       <c r="Y2" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="AA2" s="10" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -791,7 +925,7 @@
       <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="16" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -857,8 +991,11 @@
       <c r="Y3" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="AA3" s="11" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -935,7 +1072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1011,15 +1148,18 @@
       <c r="Y5" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="AA5" s="14" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -1040,7 +1180,7 @@
       <c r="I6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="16" t="s">
         <v>10</v>
       </c>
       <c r="K6" s="3" t="s">
@@ -1061,13 +1201,13 @@
       <c r="P6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Q6" s="7" t="s">
+      <c r="Q6" s="15" t="s">
         <v>6</v>
       </c>
       <c r="R6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="S6" s="7" t="s">
+      <c r="S6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="T6" s="1" t="s">
@@ -1088,8 +1228,11 @@
       <c r="Y6" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="AA6" s="19" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1165,8 +1308,11 @@
       <c r="Y7" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="AA7" s="13" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1179,7 +1325,7 @@
       <c r="D8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="15" t="s">
         <v>3</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -1242,8 +1388,11 @@
       <c r="Y8" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="AA8" s="12" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -1320,7 +1469,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1363,7 +1512,7 @@
       <c r="N10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="O10" s="7" t="s">
+      <c r="O10" s="18" t="s">
         <v>3</v>
       </c>
       <c r="P10" s="1" t="s">
@@ -1397,7 +1546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1474,7 +1623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1551,7 +1700,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1628,7 +1777,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1705,7 +1854,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1751,7 +1900,7 @@
       <c r="O15" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="P15" s="20" t="s">
         <v>0</v>
       </c>
       <c r="Q15" s="1" t="s">
@@ -1782,7 +1931,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -1795,13 +1944,13 @@
       <c r="D16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="20" t="s">
         <v>0</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="15" t="s">
         <v>5</v>
       </c>
       <c r="H16" s="1" t="s">
@@ -1816,7 +1965,7 @@
       <c r="K16" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="L16" s="17" t="s">
         <v>1</v>
       </c>
       <c r="M16" s="4" t="s">
@@ -1837,7 +1986,7 @@
       <c r="R16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="S16" s="1" t="s">
+      <c r="S16" s="22" t="s">
         <v>0</v>
       </c>
       <c r="T16" s="7" t="s">
@@ -1859,7 +2008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -1920,7 +2069,7 @@
       <c r="T17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="U17" s="7" t="s">
+      <c r="U17" s="18" t="s">
         <v>4</v>
       </c>
       <c r="V17" s="3" t="s">
@@ -1936,7 +2085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -1988,13 +2137,13 @@
       <c r="Q18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R18" s="1" t="s">
+      <c r="R18" s="21" t="s">
         <v>0</v>
       </c>
       <c r="S18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T18" s="1" t="s">
+      <c r="T18" s="20" t="s">
         <v>0</v>
       </c>
       <c r="U18" s="1" t="s">
@@ -2013,7 +2162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -2065,7 +2214,7 @@
       <c r="Q19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R19" s="1" t="s">
+      <c r="R19" s="16" t="s">
         <v>0</v>
       </c>
       <c r="S19" s="1" t="s">
@@ -2090,7 +2239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -2103,7 +2252,7 @@
       <c r="D20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="16" t="s">
         <v>19</v>
       </c>
       <c r="F20" s="3" t="s">
@@ -2167,7 +2316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -2244,17 +2393,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="7" t="s">
+      <c r="C22" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="18" t="s">
         <v>6</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -2302,7 +2451,7 @@
       <c r="S22" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="T22" s="1" t="s">
+      <c r="T22" s="22" t="s">
         <v>0</v>
       </c>
       <c r="U22" s="1" t="s">
@@ -2321,7 +2470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -2398,7 +2547,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -2475,7 +2624,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -2485,7 +2634,7 @@
       <c r="C25" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -2512,7 +2661,7 @@
       <c r="L25" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M25" s="6" t="s">
+      <c r="M25" s="18" t="s">
         <v>23</v>
       </c>
       <c r="N25" s="3" t="s">
@@ -2539,7 +2688,7 @@
       <c r="U25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="V25" s="6" t="s">
+      <c r="V25" s="18" t="s">
         <v>28</v>
       </c>
       <c r="W25" s="3" t="s">
@@ -2552,7 +2701,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -2629,7 +2778,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -2672,7 +2821,7 @@
       <c r="N27" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O27" s="1" t="s">
+      <c r="O27" s="20" t="s">
         <v>0</v>
       </c>
       <c r="P27" s="5" t="s">

</xml_diff>

<commit_message>
Pulled and fixed conflicts
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John Klassen\eclipse-workspace\ClueGameSW\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C31F935-9983-464A-A942-46E701AF4CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD155DB-050D-42CC-90AC-0A5D8E4C3C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="17550" xr2:uid="{458EB856-E50E-4072-8F58-AC2C0DAFB3C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{458EB856-E50E-4072-8F58-AC2C0DAFB3C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -371,13 +371,13 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -394,7 +394,7 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -748,7 +748,7 @@
   <dimension ref="A1:AA27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,10 +826,10 @@
         <v>21</v>
       </c>
       <c r="X1" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y1" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AA1" t="s">
         <v>35</v>

</xml_diff>